<commit_message>
Deploying to gh-pages from @ IDGRLP/Tumorkonferenzen-IG@8a458d1a37c8d2c3ec596998e75b79800875cf1d 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-HistoGradeCS.xlsx
+++ b/CodeSystem-HistoGradeCS.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-08T16:58:24+00:00</t>
+    <t>2024-05-22T07:04:28+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -69,7 +69,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>IDG Institut für digitale Gesundheitsdaten RLP gGmbH (https://www.idg-rlp.de/, info@idg-rlp.de)</t>
   </si>
   <si>
     <t>Description</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ IDGRLP/Tumorkonferenzen-IG@a6ec8440d71eb4ead340661347be820f66a9ac52 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-HistoGradeCS.xlsx
+++ b/CodeSystem-HistoGradeCS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-28T11:48:18+00:00</t>
+    <t>2024-09-17T19:55:11+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>IDG Institut für digitale Gesundheitsdaten RLP gGmbH (https://www.idg-rlp.de/, info@idg-rlp.de)</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Description</t>
@@ -335,7 +341,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -435,64 +441,72 @@
       <c r="A12" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" t="s" s="2">
+        <v>22</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s" s="2">
         <v>29</v>
       </c>
+      <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" t="s" s="2">
+        <v>31</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B21" t="s" s="2">
         <v>32</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s" s="2">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -510,171 +524,171 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D14" s="2"/>
     </row>

</xml_diff>